<commit_message>
add ncp toi_source, remove temp/sal from output
</commit_message>
<xml_diff>
--- a/ncp-gop-transect-summer-2018/discreteratesEn617.xlsx
+++ b/ncp-gop-transect-summer-2018/discreteratesEn617.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="32">
   <si>
     <t>attributeName</t>
   </si>
@@ -117,6 +117,15 @@
   </si>
   <si>
     <t>millimolePerMeterSquaredPerDay</t>
+  </si>
+  <si>
+    <t>toi_source</t>
+  </si>
+  <si>
+    <t>Bottle sample from niskin or underway</t>
+  </si>
+  <si>
+    <t>categorical</t>
   </si>
 </sst>
 </file>
@@ -479,10 +488,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="A6" sqref="A6:H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -572,30 +581,21 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" t="s">
-        <v>28</v>
-      </c>
-      <c r="F6" t="s">
-        <v>23</v>
-      </c>
-      <c r="G6" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C7" t="s">
         <v>11</v>
@@ -612,21 +612,41 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C8" t="s">
         <v>11</v>
       </c>
       <c r="D8" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="F8" t="s">
         <v>23</v>
       </c>
       <c r="G8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G9" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>